<commit_message>
feat(E2): Implement Artifact Creation Automation
- Add AI-to-Template field mapper with fuzzy matching and type coercion (F2.1)
- Add artifact preview modal for editing before creation (F2.2)
- Add batch artifact creation API with partial failure handling (F2.3)
- Add field diff viewer for change visualization (F2.4)
- Enhance artifact suggestions component with all Epic 2 features
- Update Product Roadmap with Sprint 2 completion

Features: F2.1, F2.2, F2.3, F2.4
User Stories: US-006, US-007, US-008, US-009, US-010, US-011, US-012
Test Cases: TC-003, TC-004, TC-005, TC-101, TC-102

Co-Authored-By: Claude Opus 4.5 <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/SERVE-OS-v2.0-Product-Roadmap.xlsx
+++ b/SERVE-OS-v2.0-Product-Roadmap.xlsx
@@ -582,7 +582,6 @@
         </is>
       </c>
     </row>
-    <row r="2"/>
     <row r="3">
       <c r="A3" s="2" t="inlineStr">
         <is>
@@ -597,7 +596,6 @@
         </is>
       </c>
     </row>
-    <row r="5"/>
     <row r="6">
       <c r="A6" s="2" t="inlineStr">
         <is>
@@ -707,7 +705,6 @@
         </is>
       </c>
     </row>
-    <row r="13"/>
     <row r="14">
       <c r="A14" s="2" t="inlineStr">
         <is>
@@ -869,7 +866,6 @@
         </is>
       </c>
     </row>
-    <row r="22"/>
     <row r="23">
       <c r="A23" s="2" t="inlineStr">
         <is>
@@ -1723,7 +1719,7 @@
       </c>
       <c r="J6" s="5" t="inlineStr">
         <is>
-          <t>Not Started</t>
+          <t>Complete</t>
         </is>
       </c>
     </row>
@@ -1775,7 +1771,7 @@
       </c>
       <c r="J7" s="5" t="inlineStr">
         <is>
-          <t>Not Started</t>
+          <t>Complete</t>
         </is>
       </c>
     </row>
@@ -1827,7 +1823,7 @@
       </c>
       <c r="J8" s="5" t="inlineStr">
         <is>
-          <t>Not Started</t>
+          <t>Complete</t>
         </is>
       </c>
     </row>
@@ -1879,7 +1875,7 @@
       </c>
       <c r="J9" s="5" t="inlineStr">
         <is>
-          <t>Not Started</t>
+          <t>Complete</t>
         </is>
       </c>
     </row>
@@ -7244,12 +7240,12 @@
       </c>
       <c r="H3" s="5" t="inlineStr">
         <is>
-          <t>Field mapping complexity</t>
+          <t>Complete</t>
         </is>
       </c>
       <c r="I3" s="5" t="inlineStr">
         <is>
-          <t>F1.1</t>
+          <t>2026-02-04</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Epic 3: Global Search (F3.1-F3.4)
- Add Fuse.js-based search infrastructure with fuzzy matching
- Create Command Palette UI with Cmd+K keyboard shortcut
- Implement search API endpoint with 200ms SLA tracking
- Add recent searches persistence in localStorage
- Integrate SearchProvider into dashboard layout
- Update header with search trigger and keyboard hint

Co-Authored-By: Claude Opus 4.5 <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/SERVE-OS-v2.0-Product-Roadmap.xlsx
+++ b/SERVE-OS-v2.0-Product-Roadmap.xlsx
@@ -65,7 +65,7 @@
       <sz val="12"/>
     </font>
   </fonts>
-  <fills count="11">
+  <fills count="13">
     <fill>
       <patternFill/>
     </fill>
@@ -117,6 +117,18 @@
         <fgColor rgb="00F1F5F9"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00C6EFCE"/>
+        <bgColor rgb="00C6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00FFEB9C"/>
+        <bgColor rgb="00FFEB9C"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="2">
     <border>
@@ -144,7 +156,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
@@ -194,6 +206,11 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -559,7 +576,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F28"/>
+  <dimension ref="A1:F32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -980,6 +997,42 @@
       <c r="D28" s="5" t="inlineStr">
         <is>
           <t>Client-facing capabilities</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" s="12" t="inlineStr">
+        <is>
+          <t>Development Progress</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>8 of 48 Features Complete (16.7%)</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>Sprints Complete</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>2 of 10 (20%)</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>Last Updated</t>
+        </is>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>2026-02-04 14:56</t>
         </is>
       </c>
     </row>
@@ -1391,7 +1444,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J50"/>
+  <dimension ref="A1:S50"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1462,6 +1515,16 @@
           <t>Status</t>
         </is>
       </c>
+      <c r="O1" s="12" t="inlineStr">
+        <is>
+          <t>Completion Date</t>
+        </is>
+      </c>
+      <c r="P1" s="12" t="inlineStr">
+        <is>
+          <t>Developer</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="5" t="inlineStr">
@@ -1509,9 +1572,19 @@
           <t>-</t>
         </is>
       </c>
-      <c r="J2" s="5" t="inlineStr">
+      <c r="J2" s="21" t="inlineStr">
         <is>
           <t>Complete</t>
+        </is>
+      </c>
+      <c r="O2" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="P2" t="inlineStr">
+        <is>
+          <t>Claude Opus 4.5</t>
         </is>
       </c>
     </row>
@@ -1561,9 +1634,19 @@
           <t>F1.1</t>
         </is>
       </c>
-      <c r="J3" s="5" t="inlineStr">
+      <c r="J3" s="21" t="inlineStr">
         <is>
           <t>Complete</t>
+        </is>
+      </c>
+      <c r="O3" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="P3" t="inlineStr">
+        <is>
+          <t>Claude Opus 4.5</t>
         </is>
       </c>
     </row>
@@ -1613,9 +1696,19 @@
           <t>F1.1</t>
         </is>
       </c>
-      <c r="J4" s="5" t="inlineStr">
+      <c r="J4" s="21" t="inlineStr">
         <is>
           <t>Complete</t>
+        </is>
+      </c>
+      <c r="O4" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="P4" t="inlineStr">
+        <is>
+          <t>Claude Opus 4.5</t>
         </is>
       </c>
     </row>
@@ -1665,9 +1758,19 @@
           <t>F1.1</t>
         </is>
       </c>
-      <c r="J5" s="5" t="inlineStr">
+      <c r="J5" s="21" t="inlineStr">
         <is>
           <t>Complete</t>
+        </is>
+      </c>
+      <c r="O5" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="P5" t="inlineStr">
+        <is>
+          <t>Claude Opus 4.5</t>
         </is>
       </c>
     </row>
@@ -1717,9 +1820,19 @@
           <t>F1.1</t>
         </is>
       </c>
-      <c r="J6" s="5" t="inlineStr">
+      <c r="J6" s="21" t="inlineStr">
         <is>
           <t>Complete</t>
+        </is>
+      </c>
+      <c r="O6" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="P6" t="inlineStr">
+        <is>
+          <t>Claude Opus 4.5</t>
         </is>
       </c>
     </row>
@@ -1769,9 +1882,19 @@
           <t>F2.1</t>
         </is>
       </c>
-      <c r="J7" s="5" t="inlineStr">
+      <c r="J7" s="21" t="inlineStr">
         <is>
           <t>Complete</t>
+        </is>
+      </c>
+      <c r="O7" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="P7" t="inlineStr">
+        <is>
+          <t>Claude Opus 4.5</t>
         </is>
       </c>
     </row>
@@ -1821,9 +1944,19 @@
           <t>F2.1</t>
         </is>
       </c>
-      <c r="J8" s="5" t="inlineStr">
+      <c r="J8" s="21" t="inlineStr">
         <is>
           <t>Complete</t>
+        </is>
+      </c>
+      <c r="O8" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="P8" t="inlineStr">
+        <is>
+          <t>Claude Opus 4.5</t>
         </is>
       </c>
     </row>
@@ -1873,9 +2006,19 @@
           <t>F2.2</t>
         </is>
       </c>
-      <c r="J9" s="5" t="inlineStr">
+      <c r="J9" s="21" t="inlineStr">
         <is>
           <t>Complete</t>
+        </is>
+      </c>
+      <c r="O9" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="P9" t="inlineStr">
+        <is>
+          <t>Claude Opus 4.5</t>
         </is>
       </c>
     </row>
@@ -1927,7 +2070,17 @@
       </c>
       <c r="J10" s="5" t="inlineStr">
         <is>
-          <t>Not Started</t>
+          <t>Complete</t>
+        </is>
+      </c>
+      <c r="K10" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="L10" t="inlineStr">
+        <is>
+          <t>Claude AI</t>
         </is>
       </c>
     </row>
@@ -1979,7 +2132,17 @@
       </c>
       <c r="J11" s="5" t="inlineStr">
         <is>
-          <t>Not Started</t>
+          <t>Complete</t>
+        </is>
+      </c>
+      <c r="K11" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="L11" t="inlineStr">
+        <is>
+          <t>Claude AI</t>
         </is>
       </c>
     </row>
@@ -2031,7 +2194,17 @@
       </c>
       <c r="J12" s="5" t="inlineStr">
         <is>
-          <t>Not Started</t>
+          <t>Complete</t>
+        </is>
+      </c>
+      <c r="K12" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="L12" t="inlineStr">
+        <is>
+          <t>Claude AI</t>
         </is>
       </c>
     </row>
@@ -2083,7 +2256,17 @@
       </c>
       <c r="J13" s="5" t="inlineStr">
         <is>
-          <t>Not Started</t>
+          <t>Complete</t>
+        </is>
+      </c>
+      <c r="K13" t="inlineStr">
+        <is>
+          <t>2026-02-04</t>
+        </is>
+      </c>
+      <c r="L13" t="inlineStr">
+        <is>
+          <t>Claude AI</t>
         </is>
       </c>
     </row>
@@ -7089,7 +7272,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I13"/>
+  <dimension ref="A1:J13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -7124,32 +7307,37 @@
           <t>Theme</t>
         </is>
       </c>
-      <c r="D1" s="4" t="inlineStr">
+      <c r="D1" s="12" t="inlineStr">
+        <is>
+          <t>Status</t>
+        </is>
+      </c>
+      <c r="E1" s="4" t="inlineStr">
         <is>
           <t>Features</t>
         </is>
       </c>
-      <c r="E1" s="4" t="inlineStr">
+      <c r="F1" s="4" t="inlineStr">
         <is>
           <t>Story Points</t>
         </is>
       </c>
-      <c r="F1" s="4" t="inlineStr">
+      <c r="G1" s="4" t="inlineStr">
         <is>
           <t>Capacity</t>
         </is>
       </c>
-      <c r="G1" s="4" t="inlineStr">
+      <c r="H1" s="4" t="inlineStr">
         <is>
           <t>Utilization</t>
         </is>
       </c>
-      <c r="H1" s="4" t="inlineStr">
+      <c r="I1" s="4" t="inlineStr">
         <is>
           <t>Risks</t>
         </is>
       </c>
-      <c r="I1" s="4" t="inlineStr">
+      <c r="J1" s="4" t="inlineStr">
         <is>
           <t>Dependencies</t>
         </is>
@@ -7171,32 +7359,37 @@
           <t>Foundation</t>
         </is>
       </c>
-      <c r="D2" s="5" t="inlineStr">
+      <c r="D2" s="22" t="inlineStr">
+        <is>
+          <t>Complete</t>
+        </is>
+      </c>
+      <c r="E2" s="5" t="inlineStr">
         <is>
           <t>F1.1, F1.2, F1.3, F1.4</t>
         </is>
       </c>
-      <c r="E2" s="5" t="inlineStr">
+      <c r="F2" s="5" t="inlineStr">
         <is>
           <t>16</t>
         </is>
       </c>
-      <c r="F2" s="5" t="inlineStr">
+      <c r="G2" s="5" t="inlineStr">
         <is>
           <t>20</t>
         </is>
       </c>
-      <c r="G2" s="6" t="inlineStr">
+      <c r="H2" s="6" t="inlineStr">
         <is>
           <t>80%</t>
         </is>
       </c>
-      <c r="H2" s="5" t="inlineStr">
+      <c r="I2" s="5" t="inlineStr">
         <is>
           <t>Complete</t>
         </is>
       </c>
-      <c r="I2" s="5" t="inlineStr">
+      <c r="J2" s="5" t="inlineStr">
         <is>
           <t>2026-02-04</t>
         </is>
@@ -7218,32 +7411,37 @@
           <t>Artifact Automation</t>
         </is>
       </c>
-      <c r="D3" s="5" t="inlineStr">
+      <c r="D3" s="22" t="inlineStr">
+        <is>
+          <t>Complete</t>
+        </is>
+      </c>
+      <c r="E3" s="5" t="inlineStr">
         <is>
           <t>F2.1, F2.2</t>
         </is>
       </c>
-      <c r="E3" s="5" t="inlineStr">
+      <c r="F3" s="5" t="inlineStr">
         <is>
           <t>21</t>
         </is>
       </c>
-      <c r="F3" s="5" t="inlineStr">
+      <c r="G3" s="5" t="inlineStr">
         <is>
           <t>20</t>
         </is>
       </c>
-      <c r="G3" s="10" t="inlineStr">
+      <c r="H3" s="10" t="inlineStr">
         <is>
           <t>105%</t>
         </is>
       </c>
-      <c r="H3" s="5" t="inlineStr">
+      <c r="I3" s="5" t="inlineStr">
         <is>
           <t>Complete</t>
         </is>
       </c>
-      <c r="I3" s="5" t="inlineStr">
+      <c r="J3" s="5" t="inlineStr">
         <is>
           <t>2026-02-04</t>
         </is>
@@ -7265,32 +7463,37 @@
           <t>Artifact Automation + Search</t>
         </is>
       </c>
-      <c r="D4" s="5" t="inlineStr">
+      <c r="D4" s="23" t="inlineStr">
+        <is>
+          <t>In Progress</t>
+        </is>
+      </c>
+      <c r="E4" s="5" t="inlineStr">
         <is>
           <t>F2.3, F2.4, F3.1, F3.2, F3.3, F3.4</t>
         </is>
       </c>
-      <c r="E4" s="5" t="inlineStr">
+      <c r="F4" s="5" t="inlineStr">
         <is>
           <t>29</t>
         </is>
       </c>
-      <c r="F4" s="5" t="inlineStr">
+      <c r="G4" s="5" t="inlineStr">
         <is>
           <t>30</t>
         </is>
       </c>
-      <c r="G4" s="7" t="inlineStr">
+      <c r="H4" s="7" t="inlineStr">
         <is>
           <t>97%</t>
         </is>
       </c>
-      <c r="H4" s="5" t="inlineStr">
+      <c r="I4" s="5" t="inlineStr">
         <is>
           <t>Search performance at scale</t>
         </is>
       </c>
-      <c r="I4" s="5" t="inlineStr">
+      <c r="J4" s="5" t="inlineStr">
         <is>
           <t>F2.1, DB migration</t>
         </is>
@@ -7312,32 +7515,37 @@
           <t>PDF Export</t>
         </is>
       </c>
-      <c r="D5" s="5" t="inlineStr">
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>Complete</t>
+        </is>
+      </c>
+      <c r="E5" s="5" t="inlineStr">
         <is>
           <t>F4.1, F4.2, F4.3, F4.4, F4.5, F4.6, F4.7</t>
         </is>
       </c>
-      <c r="E5" s="5" t="inlineStr">
+      <c r="F5" s="5" t="inlineStr">
         <is>
           <t>46</t>
         </is>
       </c>
-      <c r="F5" s="5" t="inlineStr">
+      <c r="G5" s="5" t="inlineStr">
         <is>
           <t>40</t>
         </is>
       </c>
-      <c r="G5" s="10" t="inlineStr">
+      <c r="H5" s="10" t="inlineStr">
         <is>
           <t>115%</t>
         </is>
       </c>
-      <c r="H5" s="5" t="inlineStr">
+      <c r="I5" s="5" t="inlineStr">
         <is>
           <t>Chart rendering in PDF</t>
         </is>
       </c>
-      <c r="I5" s="5" t="inlineStr">
+      <c r="J5" s="5" t="inlineStr">
         <is>
           <t>Storage bucket setup</t>
         </is>
@@ -7359,32 +7567,32 @@
           <t>Version Control</t>
         </is>
       </c>
-      <c r="D6" s="5" t="inlineStr">
+      <c r="E6" s="5" t="inlineStr">
         <is>
           <t>F5.1, F5.2, F5.3, F5.4, F5.5</t>
         </is>
       </c>
-      <c r="E6" s="5" t="inlineStr">
+      <c r="F6" s="5" t="inlineStr">
         <is>
           <t>31</t>
         </is>
       </c>
-      <c r="F6" s="5" t="inlineStr">
+      <c r="G6" s="5" t="inlineStr">
         <is>
           <t>30</t>
         </is>
       </c>
-      <c r="G6" s="10" t="inlineStr">
+      <c r="H6" s="10" t="inlineStr">
         <is>
           <t>103%</t>
         </is>
       </c>
-      <c r="H6" s="5" t="inlineStr">
+      <c r="I6" s="5" t="inlineStr">
         <is>
           <t>Concurrent edit edge cases</t>
         </is>
       </c>
-      <c r="I6" s="5" t="inlineStr">
+      <c r="J6" s="5" t="inlineStr">
         <is>
           <t>DB migration</t>
         </is>
@@ -7406,32 +7614,32 @@
           <t>ROI Intelligence</t>
         </is>
       </c>
-      <c r="D7" s="5" t="inlineStr">
+      <c r="E7" s="5" t="inlineStr">
         <is>
           <t>F6.1, F6.2, F6.3, F6.4, F6.5</t>
         </is>
       </c>
-      <c r="E7" s="5" t="inlineStr">
+      <c r="F7" s="5" t="inlineStr">
         <is>
           <t>36</t>
         </is>
       </c>
-      <c r="F7" s="5" t="inlineStr">
+      <c r="G7" s="5" t="inlineStr">
         <is>
           <t>30</t>
         </is>
       </c>
-      <c r="G7" s="10" t="inlineStr">
+      <c r="H7" s="10" t="inlineStr">
         <is>
           <t>120%</t>
         </is>
       </c>
-      <c r="H7" s="5" t="inlineStr">
+      <c r="I7" s="5" t="inlineStr">
         <is>
           <t>Real-time performance</t>
         </is>
       </c>
-      <c r="I7" s="5" t="inlineStr">
+      <c r="J7" s="5" t="inlineStr">
         <is>
           <t>F4.3 for PDF sync</t>
         </is>
@@ -7453,32 +7661,32 @@
           <t>Enhanced Intake</t>
         </is>
       </c>
-      <c r="D8" s="5" t="inlineStr">
+      <c r="E8" s="5" t="inlineStr">
         <is>
           <t>F7.1, F7.2, F7.3, F7.4</t>
         </is>
       </c>
-      <c r="E8" s="5" t="inlineStr">
+      <c r="F8" s="5" t="inlineStr">
         <is>
           <t>24</t>
         </is>
       </c>
-      <c r="F8" s="5" t="inlineStr">
+      <c r="G8" s="5" t="inlineStr">
         <is>
           <t>25</t>
         </is>
       </c>
-      <c r="G8" s="7" t="inlineStr">
+      <c r="H8" s="7" t="inlineStr">
         <is>
           <t>96%</t>
         </is>
       </c>
-      <c r="H8" s="5" t="inlineStr">
+      <c r="I8" s="5" t="inlineStr">
         <is>
           <t>Weighted scoring edge cases</t>
         </is>
       </c>
-      <c r="I8" s="5" t="inlineStr">
+      <c r="J8" s="5" t="inlineStr">
         <is>
           <t>DB migration</t>
         </is>
@@ -7500,32 +7708,32 @@
           <t>Template Library + Cloning</t>
         </is>
       </c>
-      <c r="D9" s="5" t="inlineStr">
+      <c r="E9" s="5" t="inlineStr">
         <is>
           <t>F8.1, F8.2, F8.3, F8.4, F9.1, F9.2, F9.3, F9.4</t>
         </is>
       </c>
-      <c r="E9" s="5" t="inlineStr">
+      <c r="F9" s="5" t="inlineStr">
         <is>
           <t>41</t>
         </is>
       </c>
-      <c r="F9" s="5" t="inlineStr">
+      <c r="G9" s="5" t="inlineStr">
         <is>
           <t>40</t>
         </is>
       </c>
-      <c r="G9" s="10" t="inlineStr">
+      <c r="H9" s="10" t="inlineStr">
         <is>
           <t>103%</t>
         </is>
       </c>
-      <c r="H9" s="5" t="inlineStr">
+      <c r="I9" s="5" t="inlineStr">
         <is>
           <t>Clone data integrity</t>
         </is>
       </c>
-      <c r="I9" s="5" t="inlineStr">
+      <c r="J9" s="5" t="inlineStr">
         <is>
           <t>None</t>
         </is>
@@ -7547,32 +7755,32 @@
           <t>Client Portal (Part 1)</t>
         </is>
       </c>
-      <c r="D10" s="5" t="inlineStr">
+      <c r="E10" s="5" t="inlineStr">
         <is>
           <t>F10.1, F10.2, F10.3, F10.4, F10.8</t>
         </is>
       </c>
-      <c r="E10" s="5" t="inlineStr">
+      <c r="F10" s="5" t="inlineStr">
         <is>
           <t>26</t>
         </is>
       </c>
-      <c r="F10" s="5" t="inlineStr">
+      <c r="G10" s="5" t="inlineStr">
         <is>
           <t>30</t>
         </is>
       </c>
-      <c r="G10" s="6" t="inlineStr">
+      <c r="H10" s="6" t="inlineStr">
         <is>
           <t>87%</t>
         </is>
       </c>
-      <c r="H10" s="5" t="inlineStr">
+      <c r="I10" s="5" t="inlineStr">
         <is>
           <t>Email deliverability</t>
         </is>
       </c>
-      <c r="I10" s="5" t="inlineStr">
+      <c r="J10" s="5" t="inlineStr">
         <is>
           <t>Email service setup</t>
         </is>
@@ -7594,49 +7802,48 @@
           <t>Client Portal (Part 2) + Polish</t>
         </is>
       </c>
-      <c r="D11" s="5" t="inlineStr">
+      <c r="E11" s="5" t="inlineStr">
         <is>
           <t>F10.5, F10.6, F10.7</t>
         </is>
       </c>
-      <c r="E11" s="5" t="inlineStr">
+      <c r="F11" s="5" t="inlineStr">
         <is>
           <t>15</t>
         </is>
       </c>
-      <c r="F11" s="5" t="inlineStr">
+      <c r="G11" s="5" t="inlineStr">
         <is>
           <t>30</t>
         </is>
       </c>
-      <c r="G11" s="6" t="inlineStr">
+      <c r="H11" s="6" t="inlineStr">
         <is>
           <t>50%</t>
         </is>
       </c>
-      <c r="H11" s="5" t="inlineStr">
+      <c r="I11" s="5" t="inlineStr">
         <is>
           <t>None - buffer for bugs</t>
         </is>
       </c>
-      <c r="I11" s="5" t="inlineStr">
+      <c r="J11" s="5" t="inlineStr">
         <is>
           <t>F10.3</t>
         </is>
       </c>
     </row>
-    <row r="12"/>
     <row r="13">
       <c r="A13" s="12" t="inlineStr">
         <is>
           <t>TOTALS</t>
         </is>
       </c>
-      <c r="E13">
+      <c r="F13">
         <f>SUM(E2:E11)</f>
         <v/>
       </c>
-      <c r="F13">
+      <c r="G13">
         <f>SUM(F2:F11)</f>
         <v/>
       </c>

</xml_diff>

<commit_message>
feat(epic-7): Add enhanced intake assessment system
- Add weighted scoring engine with category-based scoring
- Add conditional question flow with follow-up triggers
- Add pathway override with justification requirement
- Add admin weight configuration UI
- Add intake wizard with real-time score preview
- Add database migration for intake assessments

Co-Authored-By: Claude Opus 4.5 <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/SERVE-OS-v2.0-Product-Roadmap.xlsx
+++ b/SERVE-OS-v2.0-Product-Roadmap.xlsx
@@ -616,7 +616,6 @@
         </is>
       </c>
     </row>
-    <row r="2"/>
     <row r="3" ht="19" customHeight="1" s="23">
       <c r="A3" s="1" t="inlineStr">
         <is>
@@ -631,7 +630,6 @@
         </is>
       </c>
     </row>
-    <row r="5"/>
     <row r="6" ht="19" customHeight="1" s="23">
       <c r="A6" s="1" t="inlineStr">
         <is>
@@ -741,7 +739,6 @@
         </is>
       </c>
     </row>
-    <row r="13"/>
     <row r="14" ht="19" customHeight="1" s="23">
       <c r="A14" s="1" t="inlineStr">
         <is>
@@ -903,7 +900,6 @@
         </is>
       </c>
     </row>
-    <row r="22"/>
     <row r="23" ht="19" customHeight="1" s="23">
       <c r="A23" s="1" t="inlineStr">
         <is>
@@ -1021,7 +1017,6 @@
         </is>
       </c>
     </row>
-    <row r="29"/>
     <row r="30">
       <c r="A30" s="10" t="inlineStr">
         <is>
@@ -3364,7 +3359,7 @@
       </c>
       <c r="J31" s="3" t="inlineStr">
         <is>
-          <t>Not Started</t>
+          <t>Complete</t>
         </is>
       </c>
     </row>
@@ -3416,7 +3411,7 @@
       </c>
       <c r="J32" s="3" t="inlineStr">
         <is>
-          <t>Not Started</t>
+          <t>Complete</t>
         </is>
       </c>
     </row>
@@ -3468,7 +3463,7 @@
       </c>
       <c r="J33" s="3" t="inlineStr">
         <is>
-          <t>Not Started</t>
+          <t>Complete</t>
         </is>
       </c>
     </row>
@@ -3520,7 +3515,7 @@
       </c>
       <c r="J34" s="3" t="inlineStr">
         <is>
-          <t>Not Started</t>
+          <t>Complete</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
feat(epic-8): implement Template Library system (F8.1-F8.4)
- Add template library module with types, anonymizer, and examples
- Create API routes for template CRUD and usage
- Add UI components: TemplateLibrary, TemplateViewer, TemplateCard, UseTemplateDialog
- Implement PII anonymization system for template creation
- Add database migration for templates, usages, and ratings tables
- Update Product Roadmap with Epic 8 completion

User Stories: US-031, US-032

Co-Authored-By: Claude Opus 4.5 <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/SERVE-OS-v2.0-Product-Roadmap.xlsx
+++ b/SERVE-OS-v2.0-Product-Roadmap.xlsx
@@ -3567,7 +3567,17 @@
       </c>
       <c r="J35" s="3" t="inlineStr">
         <is>
-          <t>Not Started</t>
+          <t>Complete</t>
+        </is>
+      </c>
+      <c r="O35" t="inlineStr">
+        <is>
+          <t>2026-02-05</t>
+        </is>
+      </c>
+      <c r="P35" t="inlineStr">
+        <is>
+          <t>Claude Opus 4.5</t>
         </is>
       </c>
     </row>
@@ -3619,7 +3629,17 @@
       </c>
       <c r="J36" s="3" t="inlineStr">
         <is>
-          <t>Not Started</t>
+          <t>Complete</t>
+        </is>
+      </c>
+      <c r="O36" t="inlineStr">
+        <is>
+          <t>2026-02-05</t>
+        </is>
+      </c>
+      <c r="P36" t="inlineStr">
+        <is>
+          <t>Claude Opus 4.5</t>
         </is>
       </c>
     </row>
@@ -3671,7 +3691,17 @@
       </c>
       <c r="J37" s="3" t="inlineStr">
         <is>
-          <t>Not Started</t>
+          <t>Complete</t>
+        </is>
+      </c>
+      <c r="O37" t="inlineStr">
+        <is>
+          <t>2026-02-05</t>
+        </is>
+      </c>
+      <c r="P37" t="inlineStr">
+        <is>
+          <t>Claude Opus 4.5</t>
         </is>
       </c>
     </row>
@@ -3723,7 +3753,17 @@
       </c>
       <c r="J38" s="3" t="inlineStr">
         <is>
-          <t>Not Started</t>
+          <t>Complete</t>
+        </is>
+      </c>
+      <c r="O38" t="inlineStr">
+        <is>
+          <t>2026-02-05</t>
+        </is>
+      </c>
+      <c r="P38" t="inlineStr">
+        <is>
+          <t>Claude Opus 4.5</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
feat(epic-9): implement Engagement Cloning system (F9.1-F9.4)
- Add clone wizard UI with multi-step flow for engagement cloning
- Implement selective artifact cloning with client data detection
- Add client field auto-clear functionality for safe cloning
- Create clone lineage tracking with parent/child visualization
- Add database migration for engagement_clones table and RLS policies
- Update Product Roadmap with Epic 9 completion

User Stories: US-033, US-034

Co-Authored-By: Claude Opus 4.5 <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/SERVE-OS-v2.0-Product-Roadmap.xlsx
+++ b/SERVE-OS-v2.0-Product-Roadmap.xlsx
@@ -3815,7 +3815,17 @@
       </c>
       <c r="J39" s="3" t="inlineStr">
         <is>
-          <t>Not Started</t>
+          <t>Complete</t>
+        </is>
+      </c>
+      <c r="O39" t="inlineStr">
+        <is>
+          <t>2026-02-05</t>
+        </is>
+      </c>
+      <c r="P39" t="inlineStr">
+        <is>
+          <t>Claude Opus 4.5</t>
         </is>
       </c>
     </row>
@@ -3867,7 +3877,17 @@
       </c>
       <c r="J40" s="3" t="inlineStr">
         <is>
-          <t>Not Started</t>
+          <t>Complete</t>
+        </is>
+      </c>
+      <c r="O40" t="inlineStr">
+        <is>
+          <t>2026-02-05</t>
+        </is>
+      </c>
+      <c r="P40" t="inlineStr">
+        <is>
+          <t>Claude Opus 4.5</t>
         </is>
       </c>
     </row>
@@ -3919,7 +3939,17 @@
       </c>
       <c r="J41" s="3" t="inlineStr">
         <is>
-          <t>Not Started</t>
+          <t>Complete</t>
+        </is>
+      </c>
+      <c r="O41" t="inlineStr">
+        <is>
+          <t>2026-02-05</t>
+        </is>
+      </c>
+      <c r="P41" t="inlineStr">
+        <is>
+          <t>Claude Opus 4.5</t>
         </is>
       </c>
     </row>
@@ -3971,7 +4001,17 @@
       </c>
       <c r="J42" s="3" t="inlineStr">
         <is>
-          <t>Not Started</t>
+          <t>Complete</t>
+        </is>
+      </c>
+      <c r="O42" t="inlineStr">
+        <is>
+          <t>2026-02-05</t>
+        </is>
+      </c>
+      <c r="P42" t="inlineStr">
+        <is>
+          <t>Claude Opus 4.5</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
feat(epic-10): implement Client Portal with magic link authentication
- F10.1: Magic link token generation with secure hashing (SHA-256)
- F10.2: Portal session management with expiration tracking
- F10.3: Client portal dashboard with engagement overview
- F10.4: Read-only artifact viewer for client-visible deliverables
- F10.5: Progress timeline component with phase tracking
- F10.6: Artifact visibility controls (T2 sensitivity tier)
- F10.7: Portal analytics dashboard with view tracking
- F10.8: Professional HTML email templates for magic links

Database: portal_magic_links, portal_sessions, artifact_visibility,
portal_activity_log tables with RLS policies

Also includes ESLint fixes for existing components:
- artifact-preview-modal, artifact-suggestions, workflow-requirements
- info-tooltip, onboarding-checklist, workflow-guidance
- markdown-renderer

Co-Authored-By: Claude Opus 4.5 <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/SERVE-OS-v2.0-Product-Roadmap.xlsx
+++ b/SERVE-OS-v2.0-Product-Roadmap.xlsx
@@ -4063,7 +4063,17 @@
       </c>
       <c r="J43" s="3" t="inlineStr">
         <is>
-          <t>Not Started</t>
+          <t>Complete</t>
+        </is>
+      </c>
+      <c r="O43" t="inlineStr">
+        <is>
+          <t>2026-02-05</t>
+        </is>
+      </c>
+      <c r="P43" t="inlineStr">
+        <is>
+          <t>Claude Opus 4.5</t>
         </is>
       </c>
     </row>
@@ -4115,7 +4125,17 @@
       </c>
       <c r="J44" s="3" t="inlineStr">
         <is>
-          <t>Not Started</t>
+          <t>Complete</t>
+        </is>
+      </c>
+      <c r="O44" t="inlineStr">
+        <is>
+          <t>2026-02-05</t>
+        </is>
+      </c>
+      <c r="P44" t="inlineStr">
+        <is>
+          <t>Claude Opus 4.5</t>
         </is>
       </c>
     </row>
@@ -4167,7 +4187,17 @@
       </c>
       <c r="J45" s="3" t="inlineStr">
         <is>
-          <t>Not Started</t>
+          <t>Complete</t>
+        </is>
+      </c>
+      <c r="O45" t="inlineStr">
+        <is>
+          <t>2026-02-05</t>
+        </is>
+      </c>
+      <c r="P45" t="inlineStr">
+        <is>
+          <t>Claude Opus 4.5</t>
         </is>
       </c>
     </row>
@@ -4219,7 +4249,17 @@
       </c>
       <c r="J46" s="3" t="inlineStr">
         <is>
-          <t>Not Started</t>
+          <t>Complete</t>
+        </is>
+      </c>
+      <c r="O46" t="inlineStr">
+        <is>
+          <t>2026-02-05</t>
+        </is>
+      </c>
+      <c r="P46" t="inlineStr">
+        <is>
+          <t>Claude Opus 4.5</t>
         </is>
       </c>
     </row>
@@ -4271,7 +4311,17 @@
       </c>
       <c r="J47" s="3" t="inlineStr">
         <is>
-          <t>Not Started</t>
+          <t>Complete</t>
+        </is>
+      </c>
+      <c r="O47" t="inlineStr">
+        <is>
+          <t>2026-02-05</t>
+        </is>
+      </c>
+      <c r="P47" t="inlineStr">
+        <is>
+          <t>Claude Opus 4.5</t>
         </is>
       </c>
     </row>
@@ -4323,7 +4373,17 @@
       </c>
       <c r="J48" s="3" t="inlineStr">
         <is>
-          <t>Not Started</t>
+          <t>Complete</t>
+        </is>
+      </c>
+      <c r="O48" t="inlineStr">
+        <is>
+          <t>2026-02-05</t>
+        </is>
+      </c>
+      <c r="P48" t="inlineStr">
+        <is>
+          <t>Claude Opus 4.5</t>
         </is>
       </c>
     </row>
@@ -4375,7 +4435,17 @@
       </c>
       <c r="J49" s="3" t="inlineStr">
         <is>
-          <t>Not Started</t>
+          <t>Complete</t>
+        </is>
+      </c>
+      <c r="O49" t="inlineStr">
+        <is>
+          <t>2026-02-05</t>
+        </is>
+      </c>
+      <c r="P49" t="inlineStr">
+        <is>
+          <t>Claude Opus 4.5</t>
         </is>
       </c>
     </row>

</xml_diff>